<commit_message>
Template improvements and full sample.
</commit_message>
<xml_diff>
--- a/excel-flashcard-generator/src/main/resources/flashcard-template.xlsx
+++ b/excel-flashcard-generator/src/main/resources/flashcard-template.xlsx
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="180">
   <si>
     <t xml:space="preserve">${page[0].front}</t>
   </si>
@@ -80,160 +80,160 @@
     <t xml:space="preserve">${page[7].front}</t>
   </si>
   <si>
-    <t xml:space="preserve">εἷλον</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ᾑρέθην</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ᾕρηκα</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ᾕρημαι (1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">αἱρήσομαι</t>
-  </si>
-  <si>
-    <t xml:space="preserve">εἱλόμην</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ᾕρημαι (2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ἀποθανοῦμαι</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ἀπέθανον</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ἀποτέθνηκα</t>
-  </si>
-  <si>
-    <t xml:space="preserve">τέθνηκα</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ἀποκτενῶ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ἀπέκτεινα</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ἀπέκτανον</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ἀπέκτονα</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ἄρξω</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ἄρξομαι (1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ἦρξα</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ἤρχθην</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ἦρχα</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ἄρξομαι (2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ἠρξάμην</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ἦργμαι</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ἀφίξομαι</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ἀφικόμην</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ἀφῖγμαι</t>
-  </si>
-  <si>
-    <t xml:space="preserve">βήσομαι</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ἔβην</t>
-  </si>
-  <si>
-    <t xml:space="preserve">βέβηκα</t>
-  </si>
-  <si>
-    <t xml:space="preserve">γενήσομαι</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ἐγένομην</t>
-  </si>
-  <si>
-    <t xml:space="preserve">γεγένημαι</t>
-  </si>
-  <si>
-    <t xml:space="preserve">γέγονα</t>
-  </si>
-  <si>
-    <t xml:space="preserve">γνώσομαι</t>
-  </si>
-  <si>
-    <t xml:space="preserve">γνωσθήσομαι</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ἔγνων</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ἐγνώσθην</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ἔγνωκα</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ἔγνωσμαι</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ἐρωτήσω</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ἐρήσομαι</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ἐρωτηθήσομαι</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ἠρώτησα</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ἠρόμην (1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ἠρωτήθην</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ἠρώτηκα</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ἠρώτημαι</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ἠρόμην (2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ἔδομαι</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ἔφαγον</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ἠδέσθην</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ἐδήδοκα</t>
+    <t xml:space="preserve">${page[8].front}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[9].front}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[10].front}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[11].front}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[12].front}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[13].front}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[14].front}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[15].front}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[16].front}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[17].front}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[18].front}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[19].front}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[24].front}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[25].front}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[26].front}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[27].front}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[20].front}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[21].front}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[22].front}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[23].front}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[32].front}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[33].front}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[34].front}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[35].front}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[40].front}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[41].front}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[42].front}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[43].front}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[28].front}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[29].front}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[30].front}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[31].front}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[48].front}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[49].front}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[50].front}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[51].front}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[36].front}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[37].front}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[38].front}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[39].front}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[44].front}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[45].front}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[46].front}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[47].front}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[52].front}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[53].front}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[54].front}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[55].front}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[56].front}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[57].front}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[58].front}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[59].front}</t>
   </si>
   <si>
     <t xml:space="preserve">${page[3].backPrimary}</t>
@@ -284,100 +284,316 @@
     <t xml:space="preserve">${page[4].backSecondary}</t>
   </si>
   <si>
-    <t xml:space="preserve">αἱρεῖν</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pass. perfectum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">act. perfectum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pass. aorist</t>
-  </si>
-  <si>
-    <t xml:space="preserve">act. aorist</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ἀποθνῄσκειν</t>
-  </si>
-  <si>
-    <t xml:space="preserve">αἱρεῖσθαι</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sem.-dep. futurum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">med. perfectum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">med. aorist</t>
-  </si>
-  <si>
-    <t xml:space="preserve">med. futurum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ἀποκτείνειν</t>
-  </si>
-  <si>
-    <t xml:space="preserve">act. futurum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">act. perfectum (2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">act. perfectum (1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ἄρχειν</t>
-  </si>
-  <si>
-    <t xml:space="preserve">act. aorist (2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">act. aorist (1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pass. futurum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ἀφικνεῖσθαι</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ἄρχεσθαι</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dep. futurum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">βαίνειν</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dep. perfectum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dep. aorist</t>
-  </si>
-  <si>
-    <t xml:space="preserve">γίγνεσθαι</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dep. perfectum (1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">γιγνώσκειν</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dep. perfectum (2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ἐρωτᾶν</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ἐρέσθαι</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ἐσθίειν</t>
+    <t xml:space="preserve">${page[11].backPrimary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[10].backPrimary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[9].backPrimary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[8].backPrimary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[11].backSecondary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[10].backSecondary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[9].backSecondary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[8].backSecondary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[15].backPrimary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[14].backPrimary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[13].backPrimary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[12].backPrimary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[15].backSecondary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[14].backSecondary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[13].backSecondary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[12].backSecondary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[19].backPrimary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[18].backPrimary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[17].backPrimary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[16].backPrimary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[19].backSecondary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[18].backSecondary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[17].backSecondary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[16].backSecondary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[23].backPrimary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[22].backPrimary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[21].backPrimary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[20].backPrimary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[23].backSecondary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[22].backSecondary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[21].backSecondary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[20].backSecondary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[27].backPrimary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[26].backPrimary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[25].backPrimary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[24].backPrimary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[27].backSecondary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[26].backSecondary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[25].backSecondary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[24].backSecondary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[31].backPrimary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[30].backPrimary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[29].backPrimary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[28].backPrimary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[31].backSecondary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[30].backSecondary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[29].backSecondary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[28].backSecondary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[35].backPrimary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[34].backPrimary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[33].backPrimary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[32].backPrimary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[35].backSecondary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[34].backSecondary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[33].backSecondary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[32].backSecondary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[39].backPrimary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[38].backPrimary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[37].backPrimary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[36].backPrimary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[39].backSecondary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[38].backSecondary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[37].backSecondary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[36].backSecondary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[43].backPrimary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[42].backPrimary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[41].backPrimary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[40].backPrimary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[43].backSecondary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[42].backSecondary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[41].backSecondary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[40].backSecondary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[47].backPrimary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[46].backPrimary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[45].backPrimary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[44].backPrimary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[47].backSecondary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[46].backSecondary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[45].backSecondary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[44].backSecondary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[51].backPrimary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[50].backPrimary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[49].backPrimary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[48].backPrimary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[51].backSecondary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[50].backSecondary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[49].backSecondary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[48].backSecondary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[55].backPrimary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[54].backPrimary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[53].backPrimary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[52].backPrimary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[55].backSecondary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[54].backSecondary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[53].backSecondary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[52].backSecondary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[59].backPrimary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[58].backPrimary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[57].backPrimary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[56].backPrimary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[59].backSecondary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[58].backSecondary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[57].backSecondary}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${page[56].backSecondary}</t>
   </si>
 </sst>
 </file>
@@ -730,7 +946,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E64"/>
+  <dimension ref="A1:L64"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -742,7 +958,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="2" style="1" width="22.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="1.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="8.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="8" style="2" width="8.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="8.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="20.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="10" style="2" width="20.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="13" style="2" width="8.89"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -826,13 +1045,31 @@
       <c r="E8" s="4" t="s">
         <v>15</v>
       </c>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
     </row>
     <row r="9" s="1" customFormat="true" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="3"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
+      <c r="B9" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
     </row>
     <row r="10" s="1" customFormat="true" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="3"/>
@@ -848,116 +1085,211 @@
       <c r="E10" s="4" t="s">
         <v>19</v>
       </c>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
     </row>
     <row r="11" s="1" customFormat="true" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="3"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
+      <c r="B11" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
     </row>
     <row r="12" s="1" customFormat="true" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="3"/>
       <c r="B12" s="4" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>23</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
     </row>
     <row r="13" s="1" customFormat="true" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="3"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
+      <c r="B13" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
     </row>
     <row r="14" s="1" customFormat="true" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="3"/>
       <c r="B14" s="4" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>27</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
     </row>
     <row r="15" s="1" customFormat="true" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="3"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
+      <c r="B15" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
     </row>
     <row r="16" s="1" customFormat="true" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="3"/>
       <c r="B16" s="4" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>31</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
     </row>
     <row r="17" s="1" customFormat="true" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="3"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
+      <c r="B17" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
     </row>
     <row r="18" s="1" customFormat="true" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="3"/>
       <c r="B18" s="4" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>35</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
     </row>
     <row r="19" s="1" customFormat="true" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="3"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
+      <c r="B19" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
     </row>
     <row r="20" s="1" customFormat="true" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="3"/>
       <c r="B20" s="4" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>39</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
     </row>
     <row r="21" s="1" customFormat="true" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="3"/>
@@ -965,20 +1297,25 @@
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
     </row>
     <row r="22" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="3"/>
       <c r="B22" s="4" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -991,16 +1328,16 @@
     <row r="24" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="3"/>
       <c r="B24" s="4" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1013,16 +1350,16 @@
     <row r="26" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="3"/>
       <c r="B26" s="4" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1144,388 +1481,388 @@
         <v>76</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="3"/>
       <c r="B39" s="6" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="3"/>
       <c r="B40" s="5" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="3"/>
       <c r="B41" s="6" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="3"/>
       <c r="B42" s="5" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>81</v>
+        <v>93</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>81</v>
+        <v>95</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="3"/>
       <c r="B43" s="6" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="E43" s="6" t="s">
-        <v>80</v>
+        <v>99</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="3"/>
       <c r="B44" s="5" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>87</v>
+        <v>101</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>87</v>
+        <v>102</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>87</v>
+        <v>103</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="3"/>
       <c r="B45" s="6" t="s">
-        <v>88</v>
+        <v>104</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>78</v>
+        <v>105</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>92</v>
+        <v>106</v>
       </c>
       <c r="E45" s="6" t="s">
-        <v>93</v>
+        <v>107</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="3"/>
       <c r="B46" s="5" t="s">
-        <v>91</v>
+        <v>108</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>91</v>
+        <v>109</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>91</v>
+        <v>110</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>91</v>
+        <v>111</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="3"/>
       <c r="B47" s="6" t="s">
-        <v>78</v>
+        <v>112</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>79</v>
+        <v>113</v>
       </c>
       <c r="D47" s="6" t="s">
-        <v>80</v>
+        <v>114</v>
       </c>
       <c r="E47" s="6" t="s">
-        <v>94</v>
+        <v>115</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="3"/>
       <c r="B48" s="5" t="s">
-        <v>95</v>
+        <v>116</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>96</v>
+        <v>117</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>96</v>
+        <v>118</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>96</v>
+        <v>119</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="3"/>
       <c r="B49" s="6" t="s">
-        <v>97</v>
+        <v>120</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>84</v>
+        <v>121</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>85</v>
+        <v>122</v>
       </c>
       <c r="E49" s="6" t="s">
-        <v>86</v>
+        <v>123</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="3"/>
       <c r="B50" s="5" t="s">
-        <v>98</v>
+        <v>124</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>98</v>
+        <v>125</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>95</v>
+        <v>126</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>95</v>
+        <v>127</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="3"/>
       <c r="B51" s="6" t="s">
-        <v>80</v>
+        <v>128</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>83</v>
+        <v>129</v>
       </c>
       <c r="D51" s="6" t="s">
-        <v>99</v>
+        <v>130</v>
       </c>
       <c r="E51" s="6" t="s">
-        <v>100</v>
+        <v>131</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="3"/>
       <c r="B52" s="5" t="s">
-        <v>101</v>
+        <v>132</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>101</v>
+        <v>133</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>101</v>
+        <v>134</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>98</v>
+        <v>135</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="3"/>
       <c r="B53" s="6" t="s">
-        <v>102</v>
+        <v>136</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>100</v>
+        <v>137</v>
       </c>
       <c r="D53" s="6" t="s">
-        <v>97</v>
+        <v>138</v>
       </c>
       <c r="E53" s="6" t="s">
-        <v>78</v>
+        <v>139</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="3"/>
       <c r="B54" s="5" t="s">
-        <v>103</v>
+        <v>140</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>103</v>
+        <v>141</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>103</v>
+        <v>142</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>101</v>
+        <v>143</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="3"/>
       <c r="B55" s="6" t="s">
-        <v>80</v>
+        <v>144</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>94</v>
+        <v>145</v>
       </c>
       <c r="D55" s="6" t="s">
-        <v>83</v>
+        <v>146</v>
       </c>
       <c r="E55" s="6" t="s">
-        <v>104</v>
+        <v>147</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="3"/>
       <c r="B56" s="5" t="s">
-        <v>105</v>
+        <v>148</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>103</v>
+        <v>149</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>103</v>
+        <v>150</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>103</v>
+        <v>151</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="3"/>
       <c r="B57" s="6" t="s">
-        <v>88</v>
+        <v>152</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>77</v>
+        <v>153</v>
       </c>
       <c r="D57" s="6" t="s">
-        <v>78</v>
+        <v>154</v>
       </c>
       <c r="E57" s="6" t="s">
-        <v>79</v>
+        <v>155</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="3"/>
       <c r="B58" s="5" t="s">
-        <v>105</v>
+        <v>156</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>105</v>
+        <v>157</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>105</v>
+        <v>158</v>
       </c>
       <c r="E58" s="5" t="s">
-        <v>105</v>
+        <v>159</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="3"/>
       <c r="B59" s="6" t="s">
-        <v>85</v>
+        <v>160</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>80</v>
+        <v>161</v>
       </c>
       <c r="D59" s="6" t="s">
-        <v>94</v>
+        <v>162</v>
       </c>
       <c r="E59" s="6" t="s">
-        <v>86</v>
+        <v>163</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="3"/>
       <c r="B60" s="5" t="s">
-        <v>106</v>
+        <v>164</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>105</v>
+        <v>165</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>105</v>
+        <v>166</v>
       </c>
       <c r="E60" s="5" t="s">
-        <v>105</v>
+        <v>167</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="3"/>
       <c r="B61" s="6" t="s">
-        <v>100</v>
+        <v>168</v>
       </c>
       <c r="C61" s="6" t="s">
-        <v>77</v>
+        <v>169</v>
       </c>
       <c r="D61" s="6" t="s">
-        <v>78</v>
+        <v>170</v>
       </c>
       <c r="E61" s="6" t="s">
-        <v>79</v>
+        <v>171</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="3"/>
       <c r="B62" s="5" t="s">
-        <v>107</v>
+        <v>172</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>107</v>
+        <v>173</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>107</v>
+        <v>174</v>
       </c>
       <c r="E62" s="5" t="s">
-        <v>107</v>
+        <v>175</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="3"/>
       <c r="B63" s="6" t="s">
-        <v>78</v>
+        <v>176</v>
       </c>
       <c r="C63" s="6" t="s">
-        <v>79</v>
+        <v>177</v>
       </c>
       <c r="D63" s="6" t="s">
-        <v>80</v>
+        <v>178</v>
       </c>
       <c r="E63" s="6" t="s">
-        <v>83</v>
+        <v>179</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>